<commit_message>
added code to Figures.R to identify reference azo dyes in raw and calibrated data
</commit_message>
<xml_diff>
--- a/products analysis/lockmassProd2000_neg100_300_noblanks2.xlsx
+++ b/products analysis/lockmassProd2000_neg100_300_noblanks2.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Steven\Target Decoy\products analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D9B66441-6E58-4603-B775-FD95DBBA1B99}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{BF2F07C8-8C25-45C4-B19A-F93A49FE733B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="lockmassProd2000_neg300_500_nob" sheetId="1" r:id="rId1"/>
     <sheet name="Curve creation" sheetId="2" r:id="rId2"/>
+    <sheet name="Final List" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">lockmassProd2000_neg300_500_nob!$G$1:$G$1623</definedName>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="80">
   <si>
     <t>mz</t>
   </si>
@@ -3222,7 +3223,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -3787,16 +3788,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>733425</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -49915,8 +49916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AM2" sqref="AM2:AM54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -53331,4 +53332,618 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C54"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>102.01966900000001</v>
+      </c>
+      <c r="C2">
+        <v>-15.379387282696282</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>117.05572000000001</v>
+      </c>
+      <c r="C3">
+        <v>-12.130974889652473</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>121.029505</v>
+      </c>
+      <c r="C4">
+        <v>-10.782494731364141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5">
+        <v>129.01933500000001</v>
+      </c>
+      <c r="C5">
+        <v>-11.122363946573993</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6">
+        <v>129.05572000000001</v>
+      </c>
+      <c r="C6">
+        <v>-10.228140217427651</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7">
+        <v>131.03498500000001</v>
+      </c>
+      <c r="C7">
+        <v>-9.8065413598953111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <v>131.07137</v>
+      </c>
+      <c r="C8">
+        <v>-9.6893776269006064</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9">
+        <v>137.02441999999999</v>
+      </c>
+      <c r="C9">
+        <v>-8.9035224523434628</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10">
+        <v>138.01966899999999</v>
+      </c>
+      <c r="C10">
+        <v>-9.1943417135663079</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11">
+        <v>143.03498500000001</v>
+      </c>
+      <c r="C11">
+        <v>-8.9838160922361876</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12">
+        <v>143.07137</v>
+      </c>
+      <c r="C12">
+        <v>-8.8766886065689548</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13">
+        <v>145.050635</v>
+      </c>
+      <c r="C13">
+        <v>-8.5142681382147192</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14">
+        <v>145.08702</v>
+      </c>
+      <c r="C14">
+        <v>-8.408746695530315</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15">
+        <v>148.06153399999999</v>
+      </c>
+      <c r="C15">
+        <v>-7.6589777869484852</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16">
+        <v>151.04007000000001</v>
+      </c>
+      <c r="C16">
+        <v>-7.7462887828500859</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17">
+        <v>155.07137</v>
+      </c>
+      <c r="C17">
+        <v>-6.9000486679041533</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18">
+        <v>157.08702</v>
+      </c>
+      <c r="C18">
+        <v>-7.1298061417551946</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19">
+        <v>157.12340499999999</v>
+      </c>
+      <c r="C19">
+        <v>-7.6691311520316807</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20">
+        <v>165.01933500000001</v>
+      </c>
+      <c r="C20">
+        <v>-6.8779819043931614</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21">
+        <v>167.07137</v>
+      </c>
+      <c r="C21">
+        <v>-7.0029951870382803</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22">
+        <v>169.08702</v>
+      </c>
+      <c r="C22">
+        <v>-6.6238082614858378</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23">
+        <v>171.06628499999999</v>
+      </c>
+      <c r="C23">
+        <v>-6.3425706590233286</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24">
+        <v>171.10267000000002</v>
+      </c>
+      <c r="C24">
+        <v>-6.2535552485942727</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25">
+        <v>171.13905500000001</v>
+      </c>
+      <c r="C25">
+        <v>-6.7488978480764743</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26">
+        <v>173.04554999999999</v>
+      </c>
+      <c r="C26">
+        <v>-6.0677665504384475</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27">
+        <v>173.08193500000002</v>
+      </c>
+      <c r="C27">
+        <v>-6.5575878846339055</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28">
+        <v>175.06120000000001</v>
+      </c>
+      <c r="C28">
+        <v>-6.2835168501535144</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29">
+        <v>183.06628499999999</v>
+      </c>
+      <c r="C29">
+        <v>-4.8343145215542176</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30">
+        <v>185.08193500000002</v>
+      </c>
+      <c r="C30">
+        <v>-5.5921178909312426</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31">
+        <v>187.06120000000001</v>
+      </c>
+      <c r="C31">
+        <v>-4.8112596305458064</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32">
+        <v>187.09758500000001</v>
+      </c>
+      <c r="C32">
+        <v>-5.2646323575701119</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33">
+        <v>194.067014</v>
+      </c>
+      <c r="C33">
+        <v>-4.7097133158061082</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34">
+        <v>197.08193500000002</v>
+      </c>
+      <c r="C34">
+        <v>-4.2368165302591319</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35">
+        <v>199.06120000000001</v>
+      </c>
+      <c r="C35">
+        <v>-4.0188645503320446</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36">
+        <v>199.09758500000001</v>
+      </c>
+      <c r="C36">
+        <v>-4.4450564280370592</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37">
+        <v>201.07685000000001</v>
+      </c>
+      <c r="C37">
+        <v>-4.2272394858682452</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38">
+        <v>201.113235</v>
+      </c>
+      <c r="C38">
+        <v>-4.1518898544644962</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39">
+        <v>211.09758500000001</v>
+      </c>
+      <c r="C39">
+        <v>-3.7186593110839481</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40">
+        <v>213.07685000000001</v>
+      </c>
+      <c r="C40">
+        <v>-3.0505425624950195</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41">
+        <v>215.0925</v>
+      </c>
+      <c r="C41">
+        <v>-3.2544137986904045</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42">
+        <v>215.128885</v>
+      </c>
+      <c r="C42">
+        <v>-3.1841377321518936</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>67</v>
+      </c>
+      <c r="B43">
+        <v>221.08193500000002</v>
+      </c>
+      <c r="C43">
+        <v>-3.3245592862218083</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44">
+        <v>225.07685000000001</v>
+      </c>
+      <c r="C44">
+        <v>-2.4436098159541828</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45">
+        <v>227.128885</v>
+      </c>
+      <c r="C45">
+        <v>-2.5756301317683392</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46">
+        <v>239.0925</v>
+      </c>
+      <c r="C46">
+        <v>-2.5094890052657286</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47">
+        <v>239.128885</v>
+      </c>
+      <c r="C47">
+        <v>-2.446379491130676</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48">
+        <v>241.10814999999999</v>
+      </c>
+      <c r="C48">
+        <v>-1.8663823682473097</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>72</v>
+      </c>
+      <c r="B49">
+        <v>253.14453499999999</v>
+      </c>
+      <c r="C49">
+        <v>-1.7183859014841285</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>68</v>
+      </c>
+      <c r="B50">
+        <v>255.232955</v>
+      </c>
+      <c r="C50">
+        <v>-0.99908728482921105</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>259.08232999999996</v>
+      </c>
+      <c r="C51">
+        <v>-0.50177100057730173</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>265.14790699999998</v>
+      </c>
+      <c r="C52">
+        <v>-0.78069633787064374</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>73</v>
+      </c>
+      <c r="B53">
+        <v>269.13944999999995</v>
+      </c>
+      <c r="C53">
+        <v>-0.92888649336708129</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>69</v>
+      </c>
+      <c r="B54">
+        <v>283.26425499999999</v>
+      </c>
+      <c r="C54">
+        <v>-1.6062739719422199</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>